<commit_message>
Added reset switch, moved programming wires to bottom layer.
</commit_message>
<xml_diff>
--- a/atmega328p-example/minimal-atmega328p-arduino-BOM.xlsx
+++ b/atmega328p-example/minimal-atmega328p-arduino-BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56" count="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60" count="60">
   <si>
     <t>Qty</t>
   </si>
@@ -165,6 +165,15 @@
     <t>RC0805JR-070RL</t>
   </si>
   <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>RS-187R05A2-DS MT RT</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
+  </si>
+  <si>
     <t>U1</t>
   </si>
   <si>
@@ -181,6 +190,9 @@
   </si>
   <si>
     <t>ATMEGA328P-PU</t>
+  </si>
+  <si>
+    <t>X1</t>
   </si>
   <si>
     <t>ECS</t>
@@ -275,7 +287,7 @@
   <dimension ref="A1:WVT18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2181,7 +2193,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CONN HEADER VERT 6POS 2.54MM</t>
+          <t>CONN HEADER VERT 6POS 1 ROW 2.54MM</t>
         </is>
       </c>
     </row>
@@ -2214,8 +2226,10 @@
       <c r="C9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="5">
-        <v>629105136821</v>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>629105136821</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -5913,56 +5927,73 @@
       <c r="A15">
         <v>1</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SW1</t>
+        </is>
+      </c>
+      <c r="C15" t="s">
         <v>48</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>49</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>50</v>
       </c>
-      <c r="E15" t="inlineStr">
+    </row>
+    <row r="16" spans="1:16140" ht="13.5">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>IC REG LINEAR 5V 1A SOT223</t>
         </is>
       </c>
     </row>
-    <row r="16" spans="1:16140" ht="13.5">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" t="inlineStr">
+    <row r="17" spans="1:16140" ht="13.5">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>IC MCU 8BIT 32KB FLASH 28DIP</t>
         </is>
       </c>
     </row>
-    <row r="17" spans="1:16140" ht="13.5">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>X1</t>
-        </is>
-      </c>
-      <c r="C17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" t="inlineStr">
+    <row r="18" spans="1:16140" ht="13.5">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>CRYSTAL 16.000 MHZ 18PF SMD</t>
         </is>

</xml_diff>